<commit_message>
codul pentru foaia de titlu - CUATM
</commit_message>
<xml_diff>
--- a/mod_october_16/work_version.xlsx
+++ b/mod_october_16/work_version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\M3\mod_october_16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01DA13D-7F02-472B-9561-A97837D85577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F348247-E5FC-45FC-8E61-5049A2ABE984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1309,7 +1309,7 @@
     <t>CAPIa_R01_T_C11</t>
   </si>
   <si>
-    <t>SELECT LEFT(CASE WHEN TRIM(c.code) REGEXP '^[135]' AND CHAR_LENGTH(TRIM(c.code)) = 6 THEN CONCAT('0', TRIM(c.code)) ELSE TRIM(c.code) END , 4) AS code, CONCAT(LEFT(CASE WHEN TRIM(code) REGEXP '^[135]' AND CHAR_LENGTH(TRIM(code)) = 6 THEN CONCAT('0', TRIM(code)) ELSE TRIM(code) END, 4), ' - ', name) FROM taxonomy_term_data t JOIN classifier_cuatm_full c ON c.tid = t.tid  WHERE c.prgs in ('5','3','4','6','8','9') AND c.code not in ('101000');</t>
+    <t>SELECT LEFT(CASE WHEN TRIM(c.code) REGEXP '^[135]' AND CHAR_LENGTH(TRIM(c.code)) = 6 THEN CONCAT('0', TRIM(c.code)) ELSE TRIM(c.code) END , 4) AS code, CONCAT(LEFT(CASE WHEN TRIM(c.code) REGEXP '^[135]' AND CHAR_LENGTH(TRIM(c.code)) = 6 THEN CONCAT('0', TRIM(c.code)) ELSE TRIM(c.code) END, 4), ' - ',  t.name) FROM taxonomy_term_data t JOIN classifier_cuatm_full c ON c.tid = t.tid  WHERE c.prgs in ('5','3','4','6','8','9') AND c.code not in ('101000');</t>
   </si>
 </sst>
 </file>
@@ -1343,8 +1343,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1651,8 +1654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1661,6 +1664,7 @@
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
     <col min="3" max="3" width="56.42578125" customWidth="1"/>
     <col min="6" max="6" width="27.28515625" customWidth="1"/>
+    <col min="19" max="19" width="18" customWidth="1"/>
     <col min="22" max="22" width="91.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1873,7 +1877,7 @@
       <c r="R3">
         <v>0</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3" s="1" t="s">
         <v>40</v>
       </c>
       <c r="T3" t="s">

</xml_diff>